<commit_message>
Debug IntallSimplexPS.m, improve library
</commit_message>
<xml_diff>
--- a/Examples/IEEE_14Bus.xlsx
+++ b/Examples/IEEE_14Bus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Power-System-Analysis-Toolbox\Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35DCAE03-81DC-448E-8249-B4BF67B0B11B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCCD2533-6BCD-40B9-8E9A-7DF1E52D3240}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PowerFlow" sheetId="1" r:id="rId1"/>
@@ -1513,7 +1513,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34645F5B-1D7A-4323-9AD6-5FF81941CA24}">
   <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+    <sheetView topLeftCell="A21" workbookViewId="0">
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
@@ -2128,8 +2128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64D00B5E-E2E7-41B8-8388-8931D474EA96}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -2676,8 +2676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EFCB373-2341-40B6-A375-7BA50357479A}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -2767,7 +2767,7 @@
         <v>43</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" t="s">
         <v>36</v>

</xml_diff>